<commit_message>
Fix forms with custom screens
</commit_message>
<xml_diff>
--- a/app/config/tables/adult_coverage/forms/adult_coverage/adult_coverage.xlsx
+++ b/app/config/tables/adult_coverage/forms/adult_coverage/adult_coverage.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\adult_coverage\forms\adult_coverage\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7645" yWindow="2422" windowWidth="30135" windowHeight="21626" tabRatio="282" activeTab="2"/>
+    <workbookView xWindow="20320" yWindow="3820" windowWidth="30140" windowHeight="21620" tabRatio="282"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -623,9 +618,6 @@
     <t>screen.templatePath</t>
   </si>
   <si>
-    <t>../tables/adult_coverage/forms/adult_coverage/VR_adult_coverage.handlebars</t>
-  </si>
-  <si>
     <t>disableSwipeNavigation</t>
   </si>
   <si>
@@ -648,12 +640,15 @@
   </si>
   <si>
     <t>display.title.text</t>
+  </si>
+  <si>
+    <t>../config/tables/adult_coverage/forms/adult_coverage/VR_adult_coverage.handlebars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -843,7 +838,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -895,7 +890,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,34 +1118,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W104"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="9" max="9" width="35.5" customWidth="1"/>
     <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="16.875" customWidth="1"/>
-    <col min="12" max="12" width="26.375" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" customWidth="1"/>
     <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="21.125" customWidth="1"/>
-    <col min="15" max="15" width="15.875" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
     <col min="16" max="17" width="18.5" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="20" max="20" width="29.875" customWidth="1"/>
+    <col min="20" max="20" width="29.83203125" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.125" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" customWidth="1"/>
     <col min="23" max="23" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="17.5" customHeight="1">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>53</v>
@@ -1177,19 +1173,19 @@
         <v>2</v>
       </c>
       <c r="J1" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>202</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>3</v>
@@ -1207,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>8</v>
@@ -1216,10 +1212,10 @@
         <v>56</v>
       </c>
       <c r="W1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="17.5" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
@@ -1230,7 +1226,7 @@
         <v>196</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1249,7 +1245,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="17.5" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -1278,7 +1274,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="17.5" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1309,7 +1305,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1342,7 +1338,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1373,7 +1369,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1406,7 +1402,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="17.5" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1439,7 +1435,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="17.5" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1470,7 +1466,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1503,7 +1499,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="17.5" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1534,7 +1530,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1567,7 +1563,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="17.5" customHeight="1">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1600,7 +1596,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="17.5" customHeight="1">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1633,7 +1629,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="17.5" customHeight="1">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1664,7 +1660,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1697,7 +1693,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:23" ht="17.5" customHeight="1">
       <c r="G17" s="14" t="s">
         <v>65</v>
       </c>
@@ -1710,7 +1706,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G18" s="16" t="s">
         <v>144</v>
       </c>
@@ -1725,7 +1721,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:23" ht="17.5" customHeight="1">
       <c r="G19" s="17" t="s">
         <v>12</v>
       </c>
@@ -1740,7 +1736,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G20" s="14" t="s">
         <v>65</v>
       </c>
@@ -1753,7 +1749,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G21" s="16" t="s">
         <v>144</v>
       </c>
@@ -1768,7 +1764,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:23" ht="17.5" customHeight="1">
       <c r="G22" s="14" t="s">
         <v>65</v>
       </c>
@@ -1781,7 +1777,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G23" s="16" t="s">
         <v>144</v>
       </c>
@@ -1796,7 +1792,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:23" ht="17.5" customHeight="1">
       <c r="G24" s="17" t="s">
         <v>12</v>
       </c>
@@ -1811,7 +1807,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:23" ht="17.5" customHeight="1">
       <c r="G25" s="17" t="s">
         <v>12</v>
       </c>
@@ -1826,7 +1822,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:23" ht="17.5" customHeight="1">
       <c r="G26" s="14" t="s">
         <v>65</v>
       </c>
@@ -1839,7 +1835,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G27" s="16" t="s">
         <v>144</v>
       </c>
@@ -1854,7 +1850,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G28" s="17" t="s">
         <v>12</v>
       </c>
@@ -1869,7 +1865,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:23" ht="17.5" customHeight="1">
       <c r="G29" s="14" t="s">
         <v>65</v>
       </c>
@@ -1882,7 +1878,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G30" s="16" t="s">
         <v>144</v>
       </c>
@@ -1897,7 +1893,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:23" ht="17.5" customHeight="1">
       <c r="G31" s="17" t="s">
         <v>12</v>
       </c>
@@ -1912,7 +1908,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:23" ht="17.5" customHeight="1">
       <c r="G32" s="17" t="s">
         <v>12</v>
       </c>
@@ -1927,7 +1923,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:23" ht="17.5" customHeight="1">
       <c r="G33" s="14" t="s">
         <v>65</v>
       </c>
@@ -1940,7 +1936,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G34" s="16" t="s">
         <v>144</v>
       </c>
@@ -1955,7 +1951,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1974,7 +1970,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:23" ht="17.5" customHeight="1">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
@@ -1991,7 +1987,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -2010,7 +2006,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:23" ht="17.5" customHeight="1">
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -2028,7 +2024,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:23" ht="17.5" customHeight="1">
       <c r="G39" t="s">
         <v>12</v>
       </c>
@@ -2042,7 +2038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G40" s="11" t="s">
         <v>65</v>
       </c>
@@ -2053,7 +2049,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G41" s="6" t="s">
         <v>144</v>
       </c>
@@ -2067,7 +2063,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:23" ht="17.5" customHeight="1">
       <c r="G42" s="14" t="s">
         <v>65</v>
       </c>
@@ -2079,7 +2075,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G43" s="16" t="s">
         <v>144</v>
       </c>
@@ -2093,7 +2089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:23" ht="17.5" customHeight="1">
       <c r="G44" s="17" t="s">
         <v>12</v>
       </c>
@@ -2108,7 +2104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:23" ht="17.5" customHeight="1">
       <c r="G45" s="14" t="s">
         <v>65</v>
       </c>
@@ -2120,7 +2116,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G46" s="16" t="s">
         <v>144</v>
       </c>
@@ -2134,7 +2130,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:23" ht="17.5" customHeight="1">
       <c r="G47" s="17" t="s">
         <v>12</v>
       </c>
@@ -2149,7 +2145,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:23" ht="17.5" customHeight="1">
       <c r="G48" s="11" t="s">
         <v>12</v>
       </c>
@@ -2164,7 +2160,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:23" ht="17.5" customHeight="1">
       <c r="G49" s="14" t="s">
         <v>65</v>
       </c>
@@ -2176,7 +2172,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G50" s="16" t="s">
         <v>144</v>
       </c>
@@ -2190,7 +2186,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:23" ht="17.5" customHeight="1">
       <c r="G51" s="17" t="s">
         <v>12</v>
       </c>
@@ -2205,7 +2201,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:23" ht="17.5" customHeight="1">
       <c r="G52" s="14" t="s">
         <v>65</v>
       </c>
@@ -2217,7 +2213,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G53" s="16" t="s">
         <v>144</v>
       </c>
@@ -2231,7 +2227,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="54" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:23" ht="17.5" customHeight="1">
       <c r="G54" s="17" t="s">
         <v>12</v>
       </c>
@@ -2246,7 +2242,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:23" ht="17.5" customHeight="1">
       <c r="G55" s="11" t="s">
         <v>12</v>
       </c>
@@ -2261,7 +2257,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G56" s="11" t="s">
         <v>65</v>
       </c>
@@ -2272,7 +2268,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G57" s="6" t="s">
         <v>144</v>
       </c>
@@ -2286,7 +2282,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:23" ht="17.5" customHeight="1">
       <c r="G58" s="14" t="s">
         <v>65</v>
       </c>
@@ -2298,7 +2294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G59" s="16" t="s">
         <v>144</v>
       </c>
@@ -2312,7 +2308,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:23" ht="17.5" customHeight="1">
       <c r="G60" s="17" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2323,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G61" s="14" t="s">
         <v>65</v>
       </c>
@@ -2339,7 +2335,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G62" s="16" t="s">
         <v>144</v>
       </c>
@@ -2353,7 +2349,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="7:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="7:23" ht="17.5" customHeight="1">
       <c r="G63" s="14" t="s">
         <v>65</v>
       </c>
@@ -2365,7 +2361,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="7:23" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="G64" s="16" t="s">
         <v>144</v>
       </c>
@@ -2379,7 +2375,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:23" ht="17.5" customHeight="1">
       <c r="G65" s="17" t="s">
         <v>12</v>
       </c>
@@ -2394,7 +2390,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:23" ht="17.5" customHeight="1">
       <c r="G66" s="11" t="s">
         <v>12</v>
       </c>
@@ -2409,7 +2405,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:23" ht="17.5" customHeight="1">
       <c r="G67" t="s">
         <v>12</v>
       </c>
@@ -2423,7 +2419,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:23" ht="17.5" customHeight="1">
       <c r="G68" t="s">
         <v>12</v>
       </c>
@@ -2437,7 +2433,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:23" ht="17.5" customHeight="1">
       <c r="G69" t="s">
         <v>12</v>
       </c>
@@ -2451,7 +2447,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:23" ht="17.5" customHeight="1">
       <c r="G70" t="s">
         <v>12</v>
       </c>
@@ -2465,7 +2461,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:23" ht="17.5" customHeight="1">
       <c r="G71" t="s">
         <v>12</v>
       </c>
@@ -2479,7 +2475,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:23" ht="17.5" customHeight="1">
       <c r="G72" t="s">
         <v>12</v>
       </c>
@@ -2493,7 +2489,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:23" ht="17.5" customHeight="1">
       <c r="G73" t="s">
         <v>12</v>
       </c>
@@ -2507,41 +2503,41 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:23" ht="17.5" customHeight="1">
       <c r="C74" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="3:23" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:23" ht="17.5" customHeight="1"/>
+    <row r="76" spans="3:23" ht="17.5" customHeight="1"/>
+    <row r="77" spans="3:23" ht="17.5" customHeight="1"/>
+    <row r="78" spans="3:23" ht="17.5" customHeight="1"/>
+    <row r="79" spans="3:23" ht="17.5" customHeight="1"/>
+    <row r="80" spans="3:23" ht="17.5" customHeight="1"/>
+    <row r="81" ht="17.5" customHeight="1"/>
+    <row r="82" ht="17.5" customHeight="1"/>
+    <row r="83" ht="17.5" customHeight="1"/>
+    <row r="84" ht="17.5" customHeight="1"/>
+    <row r="85" ht="17.5" customHeight="1"/>
+    <row r="86" ht="17.5" customHeight="1"/>
+    <row r="87" ht="17.5" customHeight="1"/>
+    <row r="88" ht="17.5" customHeight="1"/>
+    <row r="89" ht="17.5" customHeight="1"/>
+    <row r="90" ht="17.5" customHeight="1"/>
+    <row r="91" ht="17.5" customHeight="1"/>
+    <row r="92" ht="17.5" customHeight="1"/>
+    <row r="93" ht="17.5" customHeight="1"/>
+    <row r="94" ht="17.5" customHeight="1"/>
+    <row r="95" ht="17.5" customHeight="1"/>
+    <row r="96" ht="17.5" customHeight="1"/>
+    <row r="97" ht="17.5" customHeight="1"/>
+    <row r="98" ht="17.5" customHeight="1"/>
+    <row r="99" ht="17.5" customHeight="1"/>
+    <row r="100" ht="17.5" customHeight="1"/>
+    <row r="101" ht="17.5" customHeight="1"/>
+    <row r="102" ht="17.5" customHeight="1"/>
+    <row r="103" ht="17.5" customHeight="1"/>
+    <row r="104" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2561,13 +2557,13 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.125" customWidth="1"/>
-    <col min="2" max="2" width="147.375" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="147.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -2575,7 +2571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>66</v>
       </c>
@@ -2583,7 +2579,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2591,7 +2587,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -2599,7 +2595,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2607,7 +2603,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -2615,7 +2611,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2623,7 +2619,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -2631,7 +2627,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -2639,7 +2635,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -2647,7 +2643,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2655,7 +2651,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="12.75" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>88</v>
       </c>
@@ -2663,7 +2659,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -2671,7 +2667,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -2679,7 +2675,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -2687,7 +2683,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -2695,7 +2691,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="12.75" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>96</v>
       </c>
@@ -2703,7 +2699,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="12.75" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>98</v>
       </c>
@@ -2711,7 +2707,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2719,7 +2715,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="12.75" customHeight="1">
       <c r="A20" s="11" t="s">
         <v>101</v>
       </c>
@@ -2727,7 +2723,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="12.75" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>103</v>
       </c>
@@ -2735,7 +2731,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -2743,7 +2739,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2751,7 +2747,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2759,7 +2755,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="12.75" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>109</v>
       </c>
@@ -2767,7 +2763,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="12.75" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>110</v>
       </c>
@@ -2775,7 +2771,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>112</v>
       </c>
@@ -2783,7 +2779,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -2791,7 +2787,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="12.75" customHeight="1">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2813,18 +2809,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -2832,10 +2828,10 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2846,7 +2842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2857,7 +2853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2868,7 +2864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2879,7 +2875,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2890,7 +2886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2901,7 +2897,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2912,7 +2908,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2923,7 +2919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2934,8 +2930,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2946,7 +2942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.5" customHeight="1">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2957,7 +2953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17.5" customHeight="1">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2968,7 +2964,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17.5" customHeight="1">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2979,7 +2975,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2990,7 +2986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3001,7 +2997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17.5" customHeight="1">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -3012,7 +3008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17.5" customHeight="1">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -3023,7 +3019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17.5" customHeight="1">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3034,7 +3030,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17.5" customHeight="1">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3045,8 +3041,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -3057,7 +3053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="17.5" customHeight="1">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3068,8 +3064,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="26" spans="1:3" ht="17.5" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>59</v>
       </c>
@@ -3080,7 +3076,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="12.75" customHeight="1">
       <c r="A27" s="11" t="s">
         <v>59</v>
       </c>
@@ -3091,7 +3087,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12.75" customHeight="1">
       <c r="A28" s="11" t="s">
         <v>59</v>
       </c>
@@ -3102,7 +3098,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="12.75" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>142</v>
       </c>
@@ -3131,14 +3127,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.125" customWidth="1"/>
-    <col min="3" max="3" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -3146,18 +3142,18 @@
         <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -3165,7 +3161,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>54</v>
       </c>
@@ -3173,16 +3169,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.5" customHeight="1">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>